<commit_message>
add api clear data
</commit_message>
<xml_diff>
--- a/manage/media/media.xlsx
+++ b/manage/media/media.xlsx
@@ -845,132 +845,11 @@
       </c>
       <c r="H5" s="12" t="n"/>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>QNN/LKN</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Trần Hữu Vinh</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0969981849</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Trần Hữu Vinh</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>+84915905138</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2023-12-29</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>not think</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>QNN/LKN</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Trần Hữu Vinh</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0969981849</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Trần Hữu Vinh</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>+84915905138</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2023-12-29</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>not think</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>QNN/TYA</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Trần Hữu Vinh</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0969981849</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Trần Hữu Vinh</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0969981849</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2023-12-28</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>not think</t>
-        </is>
-      </c>
-    </row>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B4:B5"/>

</xml_diff>